<commit_message>
feat: allow selecting multiple supervising lecturers
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\IPB Student Portal Logbook Bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBC9075-EFB8-4A85-8D48-4317B8E8E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCE0B90-D898-44FC-96BC-BE9D622F82E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3204" yWindow="3204" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Waktu</t>
   </si>
@@ -94,6 +94,18 @@
   </si>
   <si>
     <t>2/10/2024</t>
+  </si>
+  <si>
+    <t>Dosen</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -134,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -143,7 +155,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,24 +435,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.21875" style="2" customWidth="1"/>
     <col min="2" max="3" width="12.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="8.88671875" style="4"/>
-    <col min="6" max="6" width="14.21875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="5" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="14.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -455,19 +465,22 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
@@ -480,20 +493,23 @@
       <c r="D2" s="2">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -506,20 +522,23 @@
       <c r="D3" s="2">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -532,46 +551,49 @@
       <c r="D4" s="2">
         <v>3</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4">
         <v>0</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>